<commit_message>
Switch to author full name from initials with all downstream fixes
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests2.xlsx
+++ b/tests/testthat/testdata/struct_tests2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C3BCBC-53AB-4D3F-9C9A-04A4926CECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BEC006-3D4F-4D29-B4AD-FF8C4E33F7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21375" windowHeight="13380" xr2:uid="{EEDEB2EA-F962-40C2-B3AB-5CC011351175}"/>
+    <workbookView xWindow="2790" yWindow="2190" windowWidth="18900" windowHeight="11160" xr2:uid="{EEDEB2EA-F962-40C2-B3AB-5CC011351175}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>umar</t>
   </si>
   <si>
-    <t>mz</t>
-  </si>
-  <si>
     <t>dfg</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Maja Založnik</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -499,13 +499,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -514,19 +514,19 @@
         <v>234</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -534,13 +534,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -549,19 +549,19 @@
         <v>1123</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
         <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -569,13 +569,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -584,13 +584,13 @@
         <v>1123</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -598,13 +598,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -613,13 +613,13 @@
         <v>1123</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>